<commit_message>
feat(test): Improve code coverage.
</commit_message>
<xml_diff>
--- a/test/test_files/full-range.xlsx
+++ b/test/test_files/full-range.xlsx
@@ -8,17 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/formulas/test/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{181EED85-F218-874D-87A7-2C24234820BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62FF7315-7277-4B46-829C-74FBB1DE53D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="580" yWindow="960" windowWidth="27640" windowHeight="16000" xr2:uid="{1D9EBD42-0A85-974C-9CD8-DDEA0E8C48D6}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <definedNames>
+    <definedName name="BROKEN">[1]sheet!XFC1048576</definedName>
     <definedName name="INPUT_A">DATA!$A$2</definedName>
     <definedName name="INPUT_B">DATA!$A$3</definedName>
     <definedName name="INPUT_C">DATA!$A$4</definedName>
+    <definedName name="OUTPUT">DATA!$B$5</definedName>
   </definedNames>
   <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
@@ -94,6 +99,19 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="sheet"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -393,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA162432-7873-6F43-BE08-F17260648D9B}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -432,6 +450,12 @@
         <v>6</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <f>SUM(B2,B4,IFERROR(BROKEN,0))</f>
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat(math), #121: Improve performances of `SUMPRODUCT`, `PRODUCT`, `SUM`, and `SUMIF`.
</commit_message>
<xml_diff>
--- a/test/test_files/full-range.xlsx
+++ b/test/test_files/full-range.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/formulas/test/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62FF7315-7277-4B46-829C-74FBB1DE53D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA32BA9-CB77-F84F-93ED-AB50CA5ED77A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="580" yWindow="960" windowWidth="27640" windowHeight="16000" xr2:uid="{1D9EBD42-0A85-974C-9CD8-DDEA0E8C48D6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
     <definedName name="INPUT_C">DATA!$A$4</definedName>
     <definedName name="OUTPUT">DATA!$B$5</definedName>
   </definedNames>
-  <calcPr calcId="191029" calcOnSave="0"/>
+  <calcPr calcId="191029" iterateCount="1" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -102,7 +107,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="sheet"/>
@@ -411,15 +416,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA162432-7873-6F43-BE08-F17260648D9B}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -427,7 +432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2</v>
       </c>
@@ -435,13 +440,20 @@
         <f>SUM(A:A)</f>
         <v>13</v>
       </c>
+      <c r="C2">
+        <f>SUMPRODUCT(A:A,D:D)</f>
+        <v>38</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>5</v>
       </c>
@@ -449,11 +461,14 @@
         <f>SUM(3:3)</f>
         <v>6</v>
       </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5">
-        <f>SUM(B2,B4,IFERROR(BROKEN,0))</f>
-        <v>19</v>
+        <f>SUM(B2,B4,C2,IFERROR(BROKEN,0))</f>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix(tokens), #113: Correct `sheet_id` definition.
</commit_message>
<xml_diff>
--- a/test/test_files/full-range.xlsx
+++ b/test/test_files/full-range.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/formulas/test/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA32BA9-CB77-F84F-93ED-AB50CA5ED77A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4BEA208-B271-0644-B9B0-00154EF511E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="580" yWindow="960" windowWidth="27640" windowHeight="16000" xr2:uid="{1D9EBD42-0A85-974C-9CD8-DDEA0E8C48D6}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="1" r:id="rId1"/>
+    <sheet name="!&quot;" sheetId="2" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId2"/>
+    <externalReference r:id="rId3"/>
   </externalReferences>
   <definedNames>
     <definedName name="BROKEN">[1]sheet!XFC1048576</definedName>
@@ -419,7 +420,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -467,8 +468,28 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5">
-        <f>SUM(B2,B4,C2,IFERROR(BROKEN,0))</f>
+        <f>SUM(B2,B4,C2,'!"'!A1,IFERROR(BROKEN,0))</f>
         <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BA35D48-B2D4-2A4D-AD48-15A13137FE29}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>